<commit_message>
Added userprofile entity to the ER diagram and modified the attributes sheet
</commit_message>
<xml_diff>
--- a/TeamUp ER attributes.xlsx
+++ b/TeamUp ER attributes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>User</t>
   </si>
@@ -166,13 +166,16 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,12 +247,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,26 +346,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,23 +381,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -588,381 +557,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:C66"/>
+  <dimension ref="B2:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3">
-      <c r="B6" s="6" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="2" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="2" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="2" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="2" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="2" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="2" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="2:3">
-      <c r="B54" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3">
-      <c r="B55" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3">
-      <c r="B56" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3">
-      <c r="B59" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="2:3">
-      <c r="B60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3">
-      <c r="B61" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3">
-      <c r="B62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3">
-      <c r="B63" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3">
-      <c r="B64" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B20:C20"/>
+  <mergeCells count="8">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -975,7 +976,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -987,7 +988,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>